<commit_message>
fixed telegram selector stability using an x/y offset click
</commit_message>
<xml_diff>
--- a/GenresToVisit.xlsx
+++ b/GenresToVisit.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169C7E4B-8A1D-4B9E-801A-13327F46781A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{25CC3A7E-7270-BD4E-8BEF-EA826A40B4EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -23,6 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="14">
   <si>
     <t>Electro House</t>
   </si>
@@ -68,7 +69,7 @@
     <t>BreakBeat/Breaks</t>
   </si>
   <si>
-    <t>Mainstream</t>
+    <t>Drum &amp; Bass</t>
   </si>
 </sst>
 </file>
@@ -423,75 +424,75 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:A13"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1"/>
+    <col min="1" max="1" width="22.05859375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
Removed telegram logging and fixed many bugs
</commit_message>
<xml_diff>
--- a/GenresToVisit.xlsx
+++ b/GenresToVisit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihal\Documents\UiPath\ClandAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{25CC3A7E-7270-BD4E-8BEF-EA826A40B4EC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCDEF87-547A-4298-896B-CF76A49850D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Electro House</t>
   </si>
@@ -39,34 +39,34 @@
     <t>House</t>
   </si>
   <si>
+    <t>Deep House</t>
+  </si>
+  <si>
+    <t>Tech House</t>
+  </si>
+  <si>
+    <t>G-House</t>
+  </si>
+  <si>
+    <t>Trance</t>
+  </si>
+  <si>
+    <t>Progressive Trance</t>
+  </si>
+  <si>
+    <t>Twerk</t>
+  </si>
+  <si>
+    <t>Grime</t>
+  </si>
+  <si>
+    <t>Ambient</t>
+  </si>
+  <si>
+    <t>BreakBeat/Breaks</t>
+  </si>
+  <si>
     <t>Progressive House</t>
-  </si>
-  <si>
-    <t>Deep House</t>
-  </si>
-  <si>
-    <t>Tech House</t>
-  </si>
-  <si>
-    <t>G-House</t>
-  </si>
-  <si>
-    <t>Trance</t>
-  </si>
-  <si>
-    <t>Progressive Trance</t>
-  </si>
-  <si>
-    <t>Twerk</t>
-  </si>
-  <si>
-    <t>Grime</t>
-  </si>
-  <si>
-    <t>Ambient</t>
-  </si>
-  <si>
-    <t>BreakBeat/Breaks</t>
   </si>
   <si>
     <t>Drum &amp; Bass</t>
@@ -424,75 +424,75 @@
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.05859375" customWidth="1"/>
+    <col min="1" max="1" width="22" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
began fixing for redesign, added telegram logging framework
</commit_message>
<xml_diff>
--- a/GenresToVisit.xlsx
+++ b/GenresToVisit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihal\Documents\UiPath\ClandAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ECCDEF87-547A-4298-896B-CF76A49850D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C22F72-5925-4958-9844-7A535923C378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15990" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
+    <workbookView xWindow="-37620" yWindow="780" windowWidth="28800" windowHeight="11505" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,45 +31,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Electro House</t>
-  </si>
-  <si>
-    <t>House</t>
-  </si>
-  <si>
-    <t>Deep House</t>
-  </si>
-  <si>
-    <t>Tech House</t>
-  </si>
-  <si>
-    <t>G-House</t>
-  </si>
-  <si>
-    <t>Trance</t>
-  </si>
-  <si>
-    <t>Progressive Trance</t>
-  </si>
-  <si>
-    <t>Twerk</t>
-  </si>
-  <si>
-    <t>Grime</t>
-  </si>
-  <si>
-    <t>Ambient</t>
-  </si>
-  <si>
-    <t>BreakBeat/Breaks</t>
-  </si>
-  <si>
-    <t>Progressive House</t>
-  </si>
-  <si>
-    <t>Drum &amp; Bass</t>
   </si>
 </sst>
 </file>
@@ -421,11 +385,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862936AE-F9A5-48D0-A89B-34859B1902A0}">
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -437,66 +399,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
many changes, working version!
</commit_message>
<xml_diff>
--- a/GenresToVisit.xlsx
+++ b/GenresToVisit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mihal\Documents\UiPath\ClandAutomator\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C22F72-5925-4958-9844-7A535923C378}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E30E59-B208-471E-819D-7D2FE2C02A8E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-37620" yWindow="780" windowWidth="28800" windowHeight="11505" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
+    <workbookView xWindow="77955" yWindow="600" windowWidth="20055" windowHeight="13755" xr2:uid="{6B2788DC-6A5A-41FB-823F-D89C0DE48CB4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,9 +31,54 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>Electro House</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+  <si>
+    <t>Drum &amp; Bass</t>
+  </si>
+  <si>
+    <t>House</t>
+  </si>
+  <si>
+    <t>Trance</t>
+  </si>
+  <si>
+    <t>Techno</t>
+  </si>
+  <si>
+    <t>Nu Disco/Indie Dance</t>
+  </si>
+  <si>
+    <t>Melodic Progressive</t>
+  </si>
+  <si>
+    <t>Twerk</t>
+  </si>
+  <si>
+    <t>Ambient</t>
+  </si>
+  <si>
+    <t>Grime</t>
+  </si>
+  <si>
+    <t>BreakBeat/Breaks</t>
+  </si>
+  <si>
+    <t>Progressive House</t>
+  </si>
+  <si>
+    <t>Wave</t>
+  </si>
+  <si>
+    <t>Progressive Trance</t>
+  </si>
+  <si>
+    <t>G-House</t>
+  </si>
+  <si>
+    <t>Tech House</t>
+  </si>
+  <si>
+    <t>Deep House</t>
   </si>
 </sst>
 </file>
@@ -385,9 +430,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862936AE-F9A5-48D0-A89B-34859B1902A0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:A16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -399,6 +446,81 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>